<commit_message>
Added new CSR fmt
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/eth_csr.xlsx
+++ b/eth_csr.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6141CA-8018-AA4F-B518-E4DD8690D1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFB0DD7-90EC-8342-8246-2873E76E596C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="14940" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="16480" windowWidth="45240" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="csr_dma" sheetId="1" r:id="rId1"/>
+    <sheet name="eth_csr" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -84,12 +84,6 @@
     <t>32</t>
   </si>
   <si>
-    <t>eth_mac</t>
-  </si>
-  <si>
-    <t>Ethernet MAC address</t>
-  </si>
-  <si>
     <t>eth_ip</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
     <t>eth_csr</t>
   </si>
   <si>
-    <t>0x1DEE69DEF061</t>
-  </si>
-  <si>
     <t>0xC0A80001</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>Ethernet IP Address - Def. 192.168.0.211</t>
   </si>
   <si>
-    <t>recv_mac</t>
-  </si>
-  <si>
     <t>recv_ip</t>
   </si>
   <si>
@@ -141,9 +129,6 @@
     <t>ro</t>
   </si>
   <si>
-    <t>Received MAC addr</t>
-  </si>
-  <si>
     <t>Received IP addr</t>
   </si>
   <si>
@@ -153,18 +138,12 @@
     <t>16</t>
   </si>
   <si>
-    <t>send_mac</t>
-  </si>
-  <si>
     <t>send_ip</t>
   </si>
   <si>
     <t>send_udp_length</t>
   </si>
   <si>
-    <t>Send MAC addr</t>
-  </si>
-  <si>
     <t>Send IP addr</t>
   </si>
   <si>
@@ -181,6 +160,51 @@
   </si>
   <si>
     <t>send_pkt</t>
+  </si>
+  <si>
+    <t>eth_mac_low</t>
+  </si>
+  <si>
+    <t>0xDEF061</t>
+  </si>
+  <si>
+    <t>0x1DEE69</t>
+  </si>
+  <si>
+    <t>Ethernet MAC address - 3x LSB</t>
+  </si>
+  <si>
+    <t>Ethernet MAC address - 3x MSB</t>
+  </si>
+  <si>
+    <t>recv_mac_low</t>
+  </si>
+  <si>
+    <t>Received MAC addr - 3x LSB</t>
+  </si>
+  <si>
+    <t>Received MAC addr- 3x MSB</t>
+  </si>
+  <si>
+    <t>send_mac_low</t>
+  </si>
+  <si>
+    <t>send_mac_high</t>
+  </si>
+  <si>
+    <t>recv_mac_high</t>
+  </si>
+  <si>
+    <t>eth_mac_high</t>
+  </si>
+  <si>
+    <t>Send MAC addr - 3x LSB</t>
+  </si>
+  <si>
+    <t>Send MAC addr - 3x MSB</t>
+  </si>
+  <si>
+    <t>wotrg</t>
   </si>
 </sst>
 </file>
@@ -241,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -264,83 +288,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -400,6 +357,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -682,18 +645,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K69"/>
+  <dimension ref="B1:K72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
@@ -706,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -720,420 +683,461 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="8">
+        <v>24</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="8">
+        <v>24</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="13">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8">
+        <v>32</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="14">
+        <v>24</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="14">
+        <v>24</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="13">
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="19">
+        <v>24</v>
+      </c>
+      <c r="H14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="12" t="s">
+      <c r="I14" s="19">
+        <v>0</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="19">
+        <v>24</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="19">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0</v>
+      </c>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="19">
+        <v>0</v>
+      </c>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="21">
+        <v>0</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="21">
+        <v>0</v>
+      </c>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13">
-        <v>32</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19">
-        <v>48</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="19">
-        <v>0</v>
-      </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="19">
-        <v>0</v>
-      </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="19">
-        <v>0</v>
-      </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="24">
-        <v>48</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="24">
-        <v>0</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="24">
-        <v>0</v>
-      </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="24">
-        <v>0</v>
-      </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="24">
-        <v>0</v>
-      </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="26">
-        <v>0</v>
-      </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="26">
-        <v>0</v>
-      </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="J24"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="J25"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="J26"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27"/>
@@ -1220,12 +1224,15 @@
     <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7 G10:G11 G13:G17" numberStoredAsText="1"/>
+    <ignoredError sqref="G8 G12:G13 G16:G20" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
InFIFO working for simple burst
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/eth_csr.xlsx
+++ b/eth_csr.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFB0DD7-90EC-8342-8246-2873E76E596C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A67F8CC-FFC8-D745-B2B6-A5F728AC3E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="16480" windowWidth="45240" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11560" yWindow="8020" windowWidth="45240" windowHeight="28060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eth_csr" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -205,6 +205,87 @@
   </si>
   <si>
     <t>wotrg</t>
+  </si>
+  <si>
+    <t>send_src_port</t>
+  </si>
+  <si>
+    <t>send_dst_port</t>
+  </si>
+  <si>
+    <t>Send src port</t>
+  </si>
+  <si>
+    <t>Send dst port</t>
+  </si>
+  <si>
+    <t>recv_udp_src_port</t>
+  </si>
+  <si>
+    <t>recv_udp_dst_port</t>
+  </si>
+  <si>
+    <t>Received UDP src port</t>
+  </si>
+  <si>
+    <t>Received UDP dest port</t>
+  </si>
+  <si>
+    <t>recv_fifo_full</t>
+  </si>
+  <si>
+    <t>InFIFO Full status</t>
+  </si>
+  <si>
+    <t>recv_fifo_rd_ptr</t>
+  </si>
+  <si>
+    <t>InFIFO Read ptr</t>
+  </si>
+  <si>
+    <t>recv_fifo_wr_ptr</t>
+  </si>
+  <si>
+    <t>InFIFO Write ptr</t>
+  </si>
+  <si>
+    <t>recv_fifo_empty</t>
+  </si>
+  <si>
+    <t>InFIFO Empty status</t>
+  </si>
+  <si>
+    <t>send_fifo_full</t>
+  </si>
+  <si>
+    <t>send_fifo_rd_ptr</t>
+  </si>
+  <si>
+    <t>send_fifo_wr_ptr</t>
+  </si>
+  <si>
+    <t>send_fifo_empty</t>
+  </si>
+  <si>
+    <t>OutFIFO Full status</t>
+  </si>
+  <si>
+    <t>OutFIFO Read ptr</t>
+  </si>
+  <si>
+    <t>OutFIFO Write ptr</t>
+  </si>
+  <si>
+    <t>OutFIFO Empty status</t>
+  </si>
+  <si>
+    <t>send_fifo_clear</t>
+  </si>
+  <si>
+    <t>Clear FIFO ptrs</t>
+  </si>
+  <si>
+    <t>recv_fifo_clear</t>
   </si>
 </sst>
 </file>
@@ -260,7 +341,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,22 +373,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,19 +421,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -645,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K72"/>
+  <dimension ref="B1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -684,525 +755,809 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4">
         <v>24</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4">
         <v>24</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4">
         <v>32</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10" t="s">
+      <c r="J8" s="5"/>
+      <c r="K8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4">
         <v>32</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="10" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="14">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="10">
         <v>24</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="14">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="15" t="s">
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="14">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="10">
         <v>24</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="15" t="s">
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14" t="s">
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="14">
-        <v>0</v>
-      </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14" t="s">
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10">
+        <v>32</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10">
+        <v>32</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10">
+        <v>32</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="19">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="15">
         <v>24</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="19">
-        <v>0</v>
-      </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="20" t="s">
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="16" t="s">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="19">
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="15">
         <v>24</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="19">
-        <v>0</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="20" t="s">
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="19">
-        <v>0</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19" t="s">
+      <c r="I23" s="15">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H24" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="19">
-        <v>0</v>
-      </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19" t="s">
+      <c r="I24" s="15">
+        <v>0</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="16" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="15">
+        <v>16</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="15">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="15">
+        <v>16</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0</v>
+      </c>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15">
+        <v>32</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15">
+        <v>32</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0</v>
+      </c>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15">
+        <v>32</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="15">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="19" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="19">
-        <v>0</v>
-      </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="20" t="s">
+      <c r="H32" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="20">
+        <v>0</v>
+      </c>
+      <c r="J32" s="19"/>
+      <c r="K32" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="21" t="s">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H33" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="21">
-        <v>0</v>
-      </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21" t="s">
+      <c r="I33" s="20">
+        <v>0</v>
+      </c>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="22" t="s">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="21" t="s">
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H34" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="21">
-        <v>0</v>
-      </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="23" t="s">
+      <c r="I34" s="20">
+        <v>0</v>
+      </c>
+      <c r="J34" s="19"/>
+      <c r="K34" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="J32"/>
-    </row>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="J40"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="J42"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="J44"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="J45"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="J46"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="J48"/>
+    </row>
     <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1222,17 +1577,12 @@
     <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G8 G12:G13 G16:G20" numberStoredAsText="1"/>
+    <ignoredError sqref="G8 G14:G16 G12:G13 G23:G24 G32:G34 G27 G30 G19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update clk of logic
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/eth_csr.xlsx
+++ b/eth_csr.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEF6172-7D10-E644-9425-61DF30F8BBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD7663-C9D6-1B44-BA86-DA01AB73148D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="11620" windowWidth="45240" windowHeight="28060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="4180" windowWidth="71700" windowHeight="33100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eth_csr" sheetId="1" r:id="rId1"/>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="360" zoomScaleNormal="360" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1156,7 +1156,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>29</v>
@@ -1398,7 +1398,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Trying to add new filter port
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/eth_csr.xlsx
+++ b/eth_csr.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD7663-C9D6-1B44-BA86-DA01AB73148D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B60C394-F5EA-414A-B38B-1185C39323C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="4180" windowWidth="71700" windowHeight="33100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -153,9 +153,6 @@
     <t>clear_irq</t>
   </si>
   <si>
-    <t>Clear IRQ recv pkt</t>
-  </si>
-  <si>
     <t>Send pkt</t>
   </si>
   <si>
@@ -298,6 +295,27 @@
   </si>
   <si>
     <t>Pkt sent IRQ</t>
+  </si>
+  <si>
+    <t>recv_set_port</t>
+  </si>
+  <si>
+    <t>Once set, it only recv pkt from specific port</t>
+  </si>
+  <si>
+    <t>irq_pkt_recv_full</t>
+  </si>
+  <si>
+    <t>Recv FIFO full IRQ</t>
+  </si>
+  <si>
+    <t>Clear IRQ recv/sent pkt</t>
+  </si>
+  <si>
+    <t>recv_set_port_en</t>
+  </si>
+  <si>
+    <t>Specific port to filter</t>
   </si>
 </sst>
 </file>
@@ -327,7 +345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +388,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -398,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -466,6 +490,15 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K67"/>
+  <dimension ref="B1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="360" zoomScaleNormal="360" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:H32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -819,7 +852,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -832,16 +865,16 @@
         <v>10</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -854,11 +887,11 @@
         <v>10</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -929,7 +962,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -946,12 +979,12 @@
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -968,7 +1001,7 @@
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
@@ -1017,7 +1050,7 @@
     </row>
     <row r="14" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1034,12 +1067,12 @@
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1056,12 +1089,12 @@
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1071,19 +1104,19 @@
         <v>11</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" s="10">
         <v>0</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1100,12 +1133,12 @@
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1122,12 +1155,12 @@
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1144,12 +1177,12 @@
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1166,12 +1199,12 @@
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1188,12 +1221,12 @@
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1210,7 +1243,7 @@
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
@@ -1259,7 +1292,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -1276,12 +1309,12 @@
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -1298,12 +1331,12 @@
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -1313,19 +1346,19 @@
         <v>11</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I27" s="15">
         <v>0</v>
       </c>
       <c r="J27" s="15"/>
       <c r="K27" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -1342,12 +1375,12 @@
       </c>
       <c r="J28" s="15"/>
       <c r="K28" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -1364,12 +1397,12 @@
       </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -1386,12 +1419,12 @@
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -1408,12 +1441,12 @@
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
@@ -1423,14 +1456,14 @@
         <v>11</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I32" s="20">
         <v>0</v>
       </c>
       <c r="J32" s="19"/>
       <c r="K32" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
@@ -1445,14 +1478,14 @@
         <v>11</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I33" s="20">
         <v>0</v>
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="20" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
@@ -1467,7 +1500,7 @@
         <v>11</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I34" s="20">
         <v>0</v>
@@ -1479,7 +1512,7 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
@@ -1496,12 +1529,12 @@
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
@@ -1518,32 +1551,74 @@
       </c>
       <c r="J36" s="22"/>
       <c r="K36" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22">
+        <v>1</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="22">
+        <v>0</v>
+      </c>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="25">
+        <v>0</v>
+      </c>
+      <c r="J38" s="24"/>
+      <c r="K38" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="J37"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="J38"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="J39"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="25">
+        <v>16</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="25">
+        <v>0</v>
+      </c>
+      <c r="J39" s="24"/>
+      <c r="K39" s="26" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40"/>
@@ -1636,6 +1711,7 @@
     <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
filtered adding ip protocol
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/eth_csr.xlsx
+++ b/eth_csr.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B60C394-F5EA-414A-B38B-1185C39323C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF6723B-8018-2147-83EE-9A7131ACA989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="4180" windowWidth="71700" windowHeight="33100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="95">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -297,9 +297,6 @@
     <t>Pkt sent IRQ</t>
   </si>
   <si>
-    <t>recv_set_port</t>
-  </si>
-  <si>
     <t>Once set, it only recv pkt from specific port</t>
   </si>
   <si>
@@ -312,10 +309,19 @@
     <t>Clear IRQ recv/sent pkt</t>
   </si>
   <si>
-    <t>recv_set_port_en</t>
-  </si>
-  <si>
     <t>Specific port to filter</t>
+  </si>
+  <si>
+    <t>filter_en</t>
+  </si>
+  <si>
+    <t>filter_port</t>
+  </si>
+  <si>
+    <t>filter_ip</t>
+  </si>
+  <si>
+    <t>Specific IP to filter</t>
   </si>
 </sst>
 </file>
@@ -782,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1485,7 +1491,7 @@
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
@@ -1556,7 +1562,7 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
@@ -1573,7 +1579,7 @@
       </c>
       <c r="J37" s="22"/>
       <c r="K37" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
@@ -1595,12 +1601,12 @@
       </c>
       <c r="J38" s="24"/>
       <c r="K38" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="24" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -1617,16 +1623,30 @@
       </c>
       <c r="J39" s="24"/>
       <c r="K39" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="J40"/>
+      <c r="B40" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="25">
+        <v>32</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="25">
+        <v>0</v>
+      </c>
+      <c r="J40" s="24"/>
+      <c r="K40" s="26" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41"/>

</xml_diff>